<commit_message>
Update visulisations and code
</commit_message>
<xml_diff>
--- a/Results/training_efficency/val_hist.xlsx
+++ b/Results/training_efficency/val_hist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kang\University\MASTERARBEIT\Transformers for Imaging\Results\training_efficency\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16255C66-917B-493A-8C8A-D2C422F6EE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1732086F-E9D3-4A92-A2F3-41026238A828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5685" yWindow="2730" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>